<commit_message>
Update code be logic
</commit_message>
<xml_diff>
--- a/report/SWR302_SRD_Report0_Mapping.xlsx
+++ b/report/SWR302_SRD_Report0_Mapping.xlsx
@@ -252,9 +252,6 @@
     <t>Confirm Order</t>
   </si>
   <si>
-    <t>Validate and approve an order to shift it to the “Pending” status</t>
-  </si>
-  <si>
     <t>US-26</t>
   </si>
   <si>
@@ -644,6 +641,9 @@
   </si>
   <si>
     <t>The system shall support batch updates for product attributes (e.g., pricing, descriptions)</t>
+  </si>
+  <si>
+    <t>Validate and approve an order to shift it to the "Approved" status</t>
   </si>
 </sst>
 </file>
@@ -1111,21 +1111,85 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1135,64 +1199,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1203,18 +1215,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1507,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="28" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="AF43" sqref="AF43"/>
+    <sheetView tabSelected="1" topLeftCell="AP55" zoomScale="94" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="BC61" sqref="BC61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,64 +1530,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:51" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="B1" s="34" t="s">
+      <c r="A1" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="27" t="s">
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
-      <c r="AG1" s="27"/>
-      <c r="AH1" s="27"/>
-      <c r="AI1" s="27"/>
-      <c r="AJ1" s="27"/>
-      <c r="AK1" s="27"/>
-      <c r="AL1" s="27"/>
-      <c r="AM1" s="27"/>
-      <c r="AN1" s="27"/>
-      <c r="AO1" s="27"/>
-      <c r="AP1" s="27"/>
-      <c r="AQ1" s="27"/>
-      <c r="AR1" s="27"/>
-      <c r="AS1" s="27"/>
-      <c r="AT1" s="27"/>
-      <c r="AU1" s="27"/>
-      <c r="AV1" s="27"/>
-      <c r="AW1" s="30"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="51"/>
+      <c r="AH1" s="51"/>
+      <c r="AI1" s="51"/>
+      <c r="AJ1" s="51"/>
+      <c r="AK1" s="51"/>
+      <c r="AL1" s="51"/>
+      <c r="AM1" s="51"/>
+      <c r="AN1" s="51"/>
+      <c r="AO1" s="51"/>
+      <c r="AP1" s="51"/>
+      <c r="AQ1" s="51"/>
+      <c r="AR1" s="51"/>
+      <c r="AS1" s="51"/>
+      <c r="AT1" s="51"/>
+      <c r="AU1" s="51"/>
+      <c r="AV1" s="51"/>
+      <c r="AW1" s="52"/>
     </row>
     <row r="2" spans="1:51" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
+      <c r="A2" s="48"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>8</v>
       </c>
       <c r="K2" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L2" s="12" t="s">
         <v>11</v>
@@ -1655,88 +1655,88 @@
         <v>22</v>
       </c>
       <c r="X2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AM2" s="2" t="s">
+      <c r="AN2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AN2" s="2" t="s">
+      <c r="AO2" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="AO2" s="2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="AP2" s="2" t="s">
+      <c r="AQ2" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AQ2" s="2" t="s">
+      <c r="AR2" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AR2" s="2" t="s">
+      <c r="AS2" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="AS2" s="2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="AT2" s="2" t="s">
+      <c r="AU2" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AV2" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="AV2" s="2" t="s">
+      <c r="AW2" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="AW2" s="14" t="s">
-        <v>124</v>
-      </c>
       <c r="AX2" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:51" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1747,7 +1747,7 @@
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
       <c r="E3" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -1756,10 +1756,10 @@
       <c r="J3" s="15"/>
       <c r="K3" s="23"/>
       <c r="L3" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M3" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
@@ -1814,7 +1814,7 @@
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
       <c r="E4" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -1824,21 +1824,21 @@
       <c r="K4" s="23"/>
       <c r="L4" s="22"/>
       <c r="M4" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O4" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P4" s="15"/>
       <c r="Q4" s="15"/>
       <c r="R4" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S4" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T4" s="15"/>
       <c r="U4" s="15"/>
@@ -1887,7 +1887,7 @@
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
       <c r="E5" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -1899,16 +1899,16 @@
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
       <c r="O5" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="P5" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q5" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S5" s="15"/>
       <c r="T5" s="15"/>
@@ -1958,7 +1958,7 @@
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
@@ -1973,7 +1973,7 @@
       <c r="P6" s="15"/>
       <c r="Q6" s="15"/>
       <c r="R6" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
@@ -2023,7 +2023,7 @@
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
@@ -2039,10 +2039,10 @@
       <c r="Q7" s="15"/>
       <c r="R7" s="15"/>
       <c r="S7" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T7" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="U7" s="15"/>
       <c r="V7" s="15"/>
@@ -2087,7 +2087,7 @@
         <v>36</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -2108,7 +2108,7 @@
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
       <c r="U8" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="V8" s="15"/>
       <c r="W8" s="15"/>
@@ -2152,7 +2152,7 @@
         <v>37</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -2174,10 +2174,10 @@
       <c r="T9" s="15"/>
       <c r="U9" s="15"/>
       <c r="V9" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="W9" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X9" s="15"/>
       <c r="Y9" s="15"/>
@@ -2219,7 +2219,7 @@
         <v>38</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -2243,7 +2243,7 @@
       <c r="V10" s="15"/>
       <c r="W10" s="15"/>
       <c r="X10" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
@@ -2284,7 +2284,7 @@
         <v>39</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -2309,7 +2309,7 @@
       <c r="W11" s="15"/>
       <c r="X11" s="15"/>
       <c r="Y11" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Z11" s="15"/>
       <c r="AA11" s="15"/>
@@ -2353,7 +2353,7 @@
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
@@ -2375,10 +2375,10 @@
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
       <c r="Z12" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AA12" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AB12" s="15"/>
       <c r="AC12" s="15"/>
@@ -2420,7 +2420,7 @@
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
@@ -2443,10 +2443,10 @@
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
       <c r="AA13" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AB13" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AC13" s="15"/>
       <c r="AD13" s="15"/>
@@ -2485,7 +2485,7 @@
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -2512,10 +2512,10 @@
       <c r="AA14" s="15"/>
       <c r="AB14" s="15"/>
       <c r="AC14" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AD14" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AE14" s="15"/>
       <c r="AF14" s="15"/>
@@ -2552,7 +2552,7 @@
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -2581,7 +2581,7 @@
       <c r="AC15" s="15"/>
       <c r="AD15" s="15"/>
       <c r="AE15" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AF15" s="15"/>
       <c r="AG15" s="15"/>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -2647,7 +2647,7 @@
       <c r="AD16" s="15"/>
       <c r="AE16" s="15"/>
       <c r="AF16" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AG16" s="15"/>
       <c r="AH16" s="15"/>
@@ -2681,7 +2681,7 @@
       </c>
       <c r="B17" s="15"/>
       <c r="C17" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -2713,13 +2713,13 @@
       <c r="AE17" s="15"/>
       <c r="AF17" s="15"/>
       <c r="AG17" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AH17" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AI17" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AJ17" s="15"/>
       <c r="AK17" s="15"/>
@@ -2750,7 +2750,7 @@
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
@@ -2785,7 +2785,7 @@
       <c r="AH18" s="15"/>
       <c r="AI18" s="15"/>
       <c r="AJ18" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AK18" s="15"/>
       <c r="AL18" s="15"/>
@@ -2815,7 +2815,7 @@
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -2851,7 +2851,7 @@
       <c r="AI19" s="15"/>
       <c r="AJ19" s="15"/>
       <c r="AK19" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AL19" s="15"/>
       <c r="AM19" s="15"/>
@@ -2886,7 +2886,7 @@
       <c r="G20" s="15"/>
       <c r="H20" s="15"/>
       <c r="I20" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J20" s="15"/>
       <c r="K20" s="23"/>
@@ -2917,7 +2917,7 @@
       <c r="AJ20" s="15"/>
       <c r="AK20" s="15"/>
       <c r="AL20" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AM20" s="15"/>
       <c r="AN20" s="15"/>
@@ -2952,7 +2952,7 @@
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K21" s="23"/>
       <c r="L21" s="22"/>
@@ -2983,7 +2983,7 @@
       <c r="AK21" s="15"/>
       <c r="AL21" s="15"/>
       <c r="AM21" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AN21" s="15"/>
       <c r="AO21" s="15"/>
@@ -3014,7 +3014,7 @@
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
       <c r="G22" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
@@ -3049,7 +3049,7 @@
       <c r="AL22" s="15"/>
       <c r="AM22" s="15"/>
       <c r="AN22" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AO22" s="15"/>
       <c r="AP22" s="15"/>
@@ -3079,7 +3079,7 @@
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
       <c r="G23" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
@@ -3115,7 +3115,7 @@
       <c r="AM23" s="15"/>
       <c r="AN23" s="15"/>
       <c r="AO23" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AP23" s="15"/>
       <c r="AQ23" s="15"/>
@@ -3144,7 +3144,7 @@
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
@@ -3181,7 +3181,7 @@
       <c r="AN24" s="15"/>
       <c r="AO24" s="15"/>
       <c r="AP24" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AQ24" s="15"/>
       <c r="AR24" s="15"/>
@@ -3208,7 +3208,7 @@
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
@@ -3247,7 +3247,7 @@
       <c r="AO25" s="15"/>
       <c r="AP25" s="15"/>
       <c r="AQ25" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AR25" s="15"/>
       <c r="AS25" s="15"/>
@@ -3273,7 +3273,7 @@
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
@@ -3313,7 +3313,7 @@
       <c r="AP26" s="15"/>
       <c r="AQ26" s="15"/>
       <c r="AR26" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AS26" s="15"/>
       <c r="AT26" s="15"/>
@@ -3335,7 +3335,7 @@
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
@@ -3379,10 +3379,10 @@
       <c r="AQ27" s="15"/>
       <c r="AR27" s="15"/>
       <c r="AS27" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AT27" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AU27" s="15"/>
       <c r="AV27" s="15"/>
@@ -3398,7 +3398,7 @@
     </row>
     <row r="28" spans="1:51" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -3407,7 +3407,7 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
@@ -3448,7 +3448,7 @@
       <c r="AS28" s="15"/>
       <c r="AT28" s="15"/>
       <c r="AU28" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AV28" s="15"/>
       <c r="AW28" s="15"/>
@@ -3463,7 +3463,7 @@
     </row>
     <row r="29" spans="1:51" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -3472,7 +3472,7 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
       <c r="H29" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
@@ -3514,7 +3514,7 @@
       <c r="AT29" s="15"/>
       <c r="AU29" s="15"/>
       <c r="AV29" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AW29" s="15"/>
       <c r="AX29" s="1">
@@ -3528,7 +3528,7 @@
     </row>
     <row r="30" spans="1:51" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -3537,7 +3537,7 @@
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
       <c r="H30" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I30" s="15"/>
       <c r="J30" s="15"/>
@@ -3580,7 +3580,7 @@
       <c r="AU30" s="15"/>
       <c r="AV30" s="15"/>
       <c r="AW30" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AX30" s="1">
         <f t="shared" si="1"/>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="31" spans="1:51" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -3602,7 +3602,7 @@
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
       <c r="H31" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I31" s="15"/>
       <c r="J31" s="15"/>
@@ -3645,7 +3645,7 @@
       <c r="AU31" s="15"/>
       <c r="AV31" s="15"/>
       <c r="AW31" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AX31" s="1">
         <f t="shared" si="1"/>
@@ -3658,13 +3658,13 @@
     </row>
     <row r="32" spans="1:51" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
       <c r="E32" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
@@ -3710,7 +3710,7 @@
       <c r="AU32" s="15"/>
       <c r="AV32" s="15"/>
       <c r="AW32" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AX32" s="1">
         <f t="shared" si="1"/>
@@ -3723,7 +3723,7 @@
     </row>
     <row r="33" spans="1:61" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -3735,7 +3735,7 @@
       <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L33" s="22"/>
       <c r="M33" s="15"/>
@@ -3786,19 +3786,19 @@
     </row>
     <row r="34" spans="1:61" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:61" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="BA35" s="28" t="s">
+      <c r="BA35" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="BB35" s="53"/>
+      <c r="BC35" s="50"/>
+      <c r="BE35" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="BB35" s="31"/>
-      <c r="BC35" s="29"/>
-      <c r="BE35" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="BF35" s="29"/>
-      <c r="BH35" s="28" t="s">
+      <c r="BF35" s="50"/>
+      <c r="BH35" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="BI35" s="29"/>
+      <c r="BI35" s="50"/>
     </row>
     <row r="36" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BA36" s="9" t="s">
@@ -3814,229 +3814,229 @@
         <v>0</v>
       </c>
       <c r="BF36" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="BH36" s="3" t="s">
         <v>11</v>
       </c>
       <c r="BI36" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="33"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="33"/>
-      <c r="N37" s="33"/>
-      <c r="O37" s="33"/>
-      <c r="P37" s="33"/>
-      <c r="Q37" s="33"/>
-      <c r="R37" s="33"/>
-      <c r="S37" s="33"/>
-      <c r="T37" s="33"/>
-      <c r="U37" s="33"/>
-      <c r="V37" s="33"/>
-      <c r="W37" s="33"/>
-      <c r="X37" s="33"/>
-      <c r="Y37" s="33"/>
-      <c r="Z37" s="33"/>
-      <c r="AA37" s="33"/>
-      <c r="AB37" s="33"/>
-      <c r="AC37" s="33"/>
-      <c r="AD37" s="33"/>
-      <c r="AE37" s="33"/>
-      <c r="AH37" s="53" t="s">
-        <v>175</v>
-      </c>
-      <c r="AI37" s="54"/>
-      <c r="AJ37" s="52"/>
-      <c r="AK37" s="52"/>
-      <c r="AL37" s="52"/>
+      <c r="A37" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="B37" s="48" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="48"/>
+      <c r="K37" s="48"/>
+      <c r="L37" s="48"/>
+      <c r="M37" s="48"/>
+      <c r="N37" s="48"/>
+      <c r="O37" s="48"/>
+      <c r="P37" s="48"/>
+      <c r="Q37" s="48"/>
+      <c r="R37" s="48"/>
+      <c r="S37" s="48"/>
+      <c r="T37" s="48"/>
+      <c r="U37" s="48"/>
+      <c r="V37" s="48"/>
+      <c r="W37" s="48"/>
+      <c r="X37" s="48"/>
+      <c r="Y37" s="48"/>
+      <c r="Z37" s="48"/>
+      <c r="AA37" s="48"/>
+      <c r="AB37" s="48"/>
+      <c r="AC37" s="48"/>
+      <c r="AD37" s="48"/>
+      <c r="AE37" s="48"/>
+      <c r="AH37" s="57" t="s">
+        <v>174</v>
+      </c>
+      <c r="AI37" s="58"/>
+      <c r="AJ37" s="41"/>
+      <c r="AK37" s="41"/>
+      <c r="AL37" s="41"/>
       <c r="BA37" s="7" t="s">
         <v>26</v>
       </c>
       <c r="BB37" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="BC37" s="42" t="s">
+      <c r="BC37" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="BD37" s="41"/>
-      <c r="BE37" s="46" t="s">
+      <c r="BD37" s="30"/>
+      <c r="BE37" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="BF37" s="45" t="s">
-        <v>96</v>
+      <c r="BF37" s="34" t="s">
+        <v>95</v>
       </c>
       <c r="BH37" s="7" t="s">
         <v>12</v>
       </c>
       <c r="BI37" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
-      <c r="B38" s="37" t="s">
+      <c r="A38" s="47"/>
+      <c r="B38" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="37" t="s">
+      <c r="C38" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="E38" s="37" t="s">
+      <c r="E38" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="37" t="s">
+      <c r="F38" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="38" t="s">
+      <c r="G38" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="H38" s="37" t="s">
+      <c r="H38" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="I38" s="38" t="s">
+      <c r="I38" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="J38" s="38" t="s">
+      <c r="J38" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="K38" s="38" t="s">
+      <c r="K38" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="L38" s="38" t="s">
+      <c r="L38" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="M38" s="38" t="s">
+      <c r="M38" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="N38" s="38" t="s">
+      <c r="N38" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="O38" s="39" t="s">
+      <c r="O38" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="P38" s="39" t="s">
+      <c r="P38" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="Q38" s="39" t="s">
+      <c r="Q38" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="R38" s="39" t="s">
+      <c r="R38" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="S38" s="39" t="s">
+      <c r="S38" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="T38" s="39" t="s">
+      <c r="T38" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="U38" s="38" t="s">
+      <c r="U38" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="V38" s="37" t="s">
+      <c r="V38" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="W38" s="37" t="s">
+      <c r="W38" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="X38" s="37" t="s">
+      <c r="X38" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Y38" s="37" t="s">
+      <c r="Y38" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="Z38" s="36" t="s">
+      <c r="Z38" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="AA38" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB38" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC38" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD38" s="36" t="s">
+      <c r="AA38" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB38" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC38" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD38" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE38" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="AE38" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH38" s="55" t="s">
-        <v>176</v>
-      </c>
-      <c r="AI38" s="56"/>
-      <c r="AJ38" s="52"/>
-      <c r="AK38" s="52"/>
-      <c r="AL38" s="52"/>
+      <c r="AH38" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="AI38" s="60"/>
+      <c r="AJ38" s="41"/>
+      <c r="AK38" s="41"/>
+      <c r="AL38" s="41"/>
       <c r="BA38" s="3" t="s">
         <v>29</v>
       </c>
       <c r="BB38" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="BC38" s="43" t="s">
-        <v>190</v>
-      </c>
-      <c r="BD38" s="41"/>
-      <c r="BE38" s="47" t="s">
+      <c r="BC38" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="BD38" s="30"/>
+      <c r="BE38" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="BF38" s="45" t="s">
-        <v>95</v>
+      <c r="BF38" s="34" t="s">
+        <v>94</v>
       </c>
       <c r="BH38" s="3" t="s">
         <v>13</v>
       </c>
       <c r="BI38" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="H39" s="40" t="s">
-        <v>98</v>
+      <c r="G39" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-      <c r="N39" s="49" t="s">
-        <v>98</v>
+      <c r="N39" s="38" t="s">
+        <v>97</v>
       </c>
       <c r="O39" s="1"/>
-      <c r="P39" s="50" t="s">
-        <v>98</v>
+      <c r="P39" s="39" t="s">
+        <v>97</v>
       </c>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
@@ -4049,45 +4049,45 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
       <c r="AA39" s="1"/>
-      <c r="AB39" s="51" t="s">
-        <v>98</v>
+      <c r="AB39" s="40" t="s">
+        <v>97</v>
       </c>
       <c r="AC39" s="1"/>
       <c r="AD39" s="1"/>
       <c r="AE39" s="1"/>
-      <c r="AH39" s="57" t="s">
-        <v>177</v>
-      </c>
-      <c r="AI39" s="58"/>
-      <c r="AJ39" s="52"/>
-      <c r="AK39" s="52"/>
-      <c r="AL39" s="52"/>
+      <c r="AH39" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="AI39" s="43"/>
+      <c r="AJ39" s="41"/>
+      <c r="AK39" s="41"/>
+      <c r="AL39" s="41"/>
       <c r="BA39" s="3" t="s">
         <v>31</v>
       </c>
       <c r="BB39" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="BC39" s="44" t="s">
+      <c r="BC39" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="BD39" s="41"/>
-      <c r="BE39" s="48" t="s">
+      <c r="BD39" s="30"/>
+      <c r="BE39" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="BF39" s="45" t="s">
-        <v>94</v>
+      <c r="BF39" s="34" t="s">
+        <v>93</v>
       </c>
       <c r="BH39" s="10" t="s">
         <v>14</v>
       </c>
       <c r="BI39" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -4100,42 +4100,42 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
-      <c r="M40" s="49" t="s">
-        <v>98</v>
+      <c r="M40" s="38" t="s">
+        <v>97</v>
       </c>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
-      <c r="Q40" s="50" t="s">
-        <v>98</v>
+      <c r="Q40" s="39" t="s">
+        <v>97</v>
       </c>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
-      <c r="U40" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="V40" s="40" t="s">
-        <v>98</v>
+      <c r="U40" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="V40" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
       <c r="Y40" s="1"/>
-      <c r="Z40" s="51" t="s">
-        <v>98</v>
+      <c r="Z40" s="40" t="s">
+        <v>97</v>
       </c>
       <c r="AA40" s="1"/>
       <c r="AB40" s="1"/>
       <c r="AC40" s="1"/>
       <c r="AD40" s="1"/>
       <c r="AE40" s="1"/>
-      <c r="AH40" s="59" t="s">
-        <v>178</v>
-      </c>
-      <c r="AI40" s="60"/>
-      <c r="AJ40" s="52"/>
-      <c r="AK40" s="52"/>
-      <c r="AL40" s="52"/>
+      <c r="AH40" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="AI40" s="45"/>
+      <c r="AJ40" s="41"/>
+      <c r="AK40" s="41"/>
+      <c r="AL40" s="41"/>
       <c r="BA40" s="7" t="s">
         <v>34</v>
       </c>
@@ -4143,25 +4143,25 @@
         <v>35</v>
       </c>
       <c r="BC40" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="BD40" s="9"/>
       <c r="BE40" s="9" t="s">
         <v>4</v>
       </c>
       <c r="BF40" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BH40" s="3" t="s">
         <v>15</v>
       </c>
       <c r="BI40" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="41" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -4170,8 +4170,8 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="49" t="s">
-        <v>98</v>
+      <c r="I41" s="38" t="s">
+        <v>97</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -4181,69 +4181,69 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
-      <c r="R41" s="50" t="s">
-        <v>98</v>
+      <c r="R41" s="39" t="s">
+        <v>97</v>
       </c>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
-      <c r="X41" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y41" s="40" t="s">
-        <v>98</v>
+      <c r="X41" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y41" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="Z41" s="1"/>
       <c r="AA41" s="1"/>
       <c r="AB41" s="1"/>
       <c r="AC41" s="1"/>
       <c r="AD41" s="1"/>
-      <c r="AE41" s="51" t="s">
-        <v>98</v>
+      <c r="AE41" s="40" t="s">
+        <v>97</v>
       </c>
       <c r="BA41" s="3" t="s">
         <v>36</v>
       </c>
       <c r="BB41" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BC41" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BE41" s="7" t="s">
         <v>5</v>
       </c>
       <c r="BF41" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="BH41" s="7" t="s">
         <v>16</v>
       </c>
       <c r="BI41" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B42" s="40" t="s">
-        <v>98</v>
+        <v>172</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="40" t="s">
-        <v>98</v>
+      <c r="F42" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="49" t="s">
-        <v>98</v>
+      <c r="K42" s="38" t="s">
+        <v>97</v>
       </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -4252,8 +4252,8 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
-      <c r="S42" s="50" t="s">
-        <v>98</v>
+      <c r="S42" s="39" t="s">
+        <v>97</v>
       </c>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
@@ -4264,8 +4264,8 @@
       <c r="Z42" s="1"/>
       <c r="AA42" s="1"/>
       <c r="AB42" s="1"/>
-      <c r="AC42" s="51" t="s">
-        <v>98</v>
+      <c r="AC42" s="40" t="s">
+        <v>97</v>
       </c>
       <c r="AD42" s="1"/>
       <c r="AE42" s="1"/>
@@ -4273,35 +4273,35 @@
         <v>37</v>
       </c>
       <c r="BB42" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="BC42" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="BE42" s="3" t="s">
         <v>6</v>
       </c>
       <c r="BF42" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BH42" s="3" t="s">
         <v>17</v>
       </c>
       <c r="BI42" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B43" s="1"/>
-      <c r="C43" s="40" t="s">
-        <v>98</v>
+      <c r="C43" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="D43" s="1"/>
-      <c r="E43" s="40" t="s">
-        <v>98</v>
+      <c r="E43" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -4309,13 +4309,13 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="49" t="s">
-        <v>98</v>
+      <c r="L43" s="38" t="s">
+        <v>97</v>
       </c>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
-      <c r="O43" s="50" t="s">
-        <v>98</v>
+      <c r="O43" s="39" t="s">
+        <v>97</v>
       </c>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
@@ -4328,8 +4328,8 @@
       <c r="X43" s="1"/>
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
-      <c r="AA43" s="51" t="s">
-        <v>98</v>
+      <c r="AA43" s="40" t="s">
+        <v>97</v>
       </c>
       <c r="AB43" s="1"/>
       <c r="AC43" s="1"/>
@@ -4339,40 +4339,40 @@
         <v>38</v>
       </c>
       <c r="BB43" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BC43" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="BE43" s="7" t="s">
         <v>7</v>
       </c>
       <c r="BF43" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="BH43" s="7" t="s">
         <v>18</v>
       </c>
       <c r="BI43" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="40" t="s">
-        <v>98</v>
+      <c r="D44" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="49" t="s">
-        <v>98</v>
+      <c r="J44" s="38" t="s">
+        <v>97</v>
       </c>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -4383,13 +4383,13 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
-      <c r="T44" s="50" t="s">
-        <v>98</v>
+      <c r="T44" s="39" t="s">
+        <v>97</v>
       </c>
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
-      <c r="W44" s="40" t="s">
-        <v>98</v>
+      <c r="W44" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="X44" s="1"/>
       <c r="Y44" s="1"/>
@@ -4397,8 +4397,8 @@
       <c r="AA44" s="1"/>
       <c r="AB44" s="1"/>
       <c r="AC44" s="1"/>
-      <c r="AD44" s="51" t="s">
-        <v>98</v>
+      <c r="AD44" s="40" t="s">
+        <v>97</v>
       </c>
       <c r="AE44" s="1"/>
       <c r="BA44" s="3" t="s">
@@ -4408,19 +4408,19 @@
         <v>40</v>
       </c>
       <c r="BC44" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="BE44" s="3" t="s">
         <v>8</v>
       </c>
       <c r="BF44" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="BH44" s="3" t="s">
         <v>19</v>
       </c>
       <c r="BI44" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4428,22 +4428,22 @@
         <v>41</v>
       </c>
       <c r="BB45" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BC45" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="BE45" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="BF45" s="11" t="s">
         <v>89</v>
-      </c>
-      <c r="BF45" s="11" t="s">
-        <v>90</v>
       </c>
       <c r="BH45" s="7" t="s">
         <v>20</v>
       </c>
       <c r="BI45" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4454,13 +4454,13 @@
         <v>43</v>
       </c>
       <c r="BC46" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="BH46" s="3" t="s">
         <v>21</v>
       </c>
       <c r="BI46" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4468,16 +4468,16 @@
         <v>44</v>
       </c>
       <c r="BB47" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="BC47" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="BH47" s="7" t="s">
         <v>22</v>
       </c>
       <c r="BI47" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4491,10 +4491,10 @@
         <v>47</v>
       </c>
       <c r="BH48" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="BI48" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4508,10 +4508,10 @@
         <v>50</v>
       </c>
       <c r="BH49" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BI49" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4525,10 +4525,10 @@
         <v>53</v>
       </c>
       <c r="BH50" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BI50" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4542,10 +4542,10 @@
         <v>56</v>
       </c>
       <c r="BH51" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BI51" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4556,13 +4556,13 @@
         <v>58</v>
       </c>
       <c r="BC52" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="BH52" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="BI52" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4573,13 +4573,13 @@
         <v>60</v>
       </c>
       <c r="BC53" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BH53" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BI53" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4593,10 +4593,10 @@
         <v>63</v>
       </c>
       <c r="BH54" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="BI54" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4610,10 +4610,10 @@
         <v>66</v>
       </c>
       <c r="BH55" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BI55" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="56" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4627,10 +4627,10 @@
         <v>69</v>
       </c>
       <c r="BH56" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BI56" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4644,10 +4644,10 @@
         <v>72</v>
       </c>
       <c r="BH57" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BI57" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4655,16 +4655,16 @@
         <v>73</v>
       </c>
       <c r="BB58" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="BC58" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="BH58" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="BI58" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4672,16 +4672,16 @@
         <v>74</v>
       </c>
       <c r="BB59" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="BC59" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BH59" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="BI59" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="60" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4692,185 +4692,185 @@
         <v>76</v>
       </c>
       <c r="BC60" s="8" t="s">
-        <v>77</v>
+        <v>207</v>
       </c>
       <c r="BH60" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="BI60" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BA61" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="BB61" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="BB61" s="8" t="s">
+      <c r="BC61" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="BC61" s="8" t="s">
-        <v>80</v>
-      </c>
       <c r="BH61" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="BI61" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BA62" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="BB62" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="BB62" s="8" t="s">
+      <c r="BC62" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="BC62" s="8" t="s">
-        <v>83</v>
-      </c>
       <c r="BH62" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="BI62" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BA63" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="BB63" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="BC63" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="BB63" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="BC63" s="8" t="s">
-        <v>85</v>
-      </c>
       <c r="BH63" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="BI63" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BA64" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="BB64" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BC64" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BH64" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="BI64" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BA65" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="BB65" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="BC65" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="BH65" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="BI65" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="66" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BA66" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BB66" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="BC66" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="BH66" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="BI66" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BH67" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="BI67" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="68" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BH68" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="BI68" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BH69" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="BI69" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BH70" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="BI70" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BH71" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="BI71" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="72" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BH72" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="BI72" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" spans="53:61" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BH73" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BI73" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="BH35:BI35"/>
+    <mergeCell ref="L1:AW1"/>
+    <mergeCell ref="BA35:BC35"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:K1"/>
     <mergeCell ref="AH39:AI39"/>
     <mergeCell ref="AH40:AI40"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="B37:AE37"/>
     <mergeCell ref="BE35:BF35"/>
-    <mergeCell ref="BH35:BI35"/>
-    <mergeCell ref="L1:AW1"/>
-    <mergeCell ref="BA35:BC35"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:K1"/>
     <mergeCell ref="AH37:AI37"/>
     <mergeCell ref="AH38:AI38"/>
   </mergeCells>

</xml_diff>